<commit_message>
Update Koffi benchmark results and instructions
</commit_message>
<xml_diff>
--- a/web/koffi.dev/benchmarks.xlsx
+++ b/web/koffi.dev/benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\luigi\koffi\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\rygel\web\koffi.dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4212C7-5550-47AA-94B5-384CF4684232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058FF10C-74D1-4197-9AD6-4258F55E2EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25425" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
+    <workbookView xWindow="2430" yWindow="420" windowWidth="23850" windowHeight="14760" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.76</c:v>
+                          <c:v>× 0.61</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -719,7 +719,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.68</c:v>
+                          <c:v>× 0.59</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -763,7 +763,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.006</c:v>
+                          <c:v>× 0.008</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -851,7 +851,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.83</c:v>
+                          <c:v>× 0.94</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -895,7 +895,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.28</c:v>
+                          <c:v>× 0.3</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1029,7 +1029,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.02</c:v>
@@ -1038,19 +1038,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.68</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.83</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,7 +1724,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.76</c:v>
+                          <c:v>× 0.64</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1856,7 +1856,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.65</c:v>
+                          <c:v>× 0.55</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1900,7 +1900,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.008</c:v>
+                          <c:v>× 0.01</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1988,7 +1988,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.83</c:v>
+                          <c:v>× 0.92</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2032,7 +2032,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.23</c:v>
+                          <c:v>× 0.28</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2166,7 +2166,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.02</c:v>
@@ -2175,19 +2175,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.65</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.83</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.23</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3822,8 +3822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CCB824-727A-454B-9045-C9B1F28AEFCD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3864,11 +3864,11 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.76</v>
+        <v>0.61</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C4, ",", "."))</f>
-        <v>× 0.76</v>
+        <v>× 0.61</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3911,11 +3911,11 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
       <c r="D8" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C8, ",", "."))</f>
-        <v>× 0.68</v>
+        <v>× 0.59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3924,11 +3924,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D9" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C9, ",", "."))</f>
-        <v>× 0.006</v>
+        <v>× 0.008</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3958,11 +3958,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>0.83</v>
+        <v>0.94</v>
       </c>
       <c r="D12" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C12, ",", "."))</f>
-        <v>× 0.83</v>
+        <v>× 0.94</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,11 +3971,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="D13" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C13, ",", "."))</f>
-        <v>× 0.28</v>
+        <v>× 0.3</v>
       </c>
     </row>
   </sheetData>
@@ -3989,8 +3989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF254FDB-3299-431D-8033-6BEFA204D913}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4031,11 +4031,11 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C4, ",", "."))</f>
-        <v>× 0.76</v>
+        <v>× 0.64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4078,11 +4078,11 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>0.65</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D8" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C8, ",", "."))</f>
-        <v>× 0.65</v>
+        <v>× 0.55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,11 +4091,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D9" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C9, ",", "."))</f>
-        <v>× 0.008</v>
+        <v>× 0.01</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4125,11 +4125,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>0.83</v>
+        <v>0.92</v>
       </c>
       <c r="D12" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C12, ",", "."))</f>
-        <v>× 0.83</v>
+        <v>× 0.92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4138,11 +4138,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>0.23</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D13" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C13, ",", "."))</f>
-        <v>× 0.23</v>
+        <v>× 0.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>